<commit_message>
Modificación Login y Modificar empresas
</commit_message>
<xml_diff>
--- a/TEMP/EMPRESA_998/MODULOS DE SUBCUENTA DE BLOQUE.xlsx
+++ b/TEMP/EMPRESA_998/MODULOS DE SUBCUENTA DE BLOQUE.xlsx
@@ -15,9 +15,151 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>VACA PRIETO WALTER JALIL</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="true"/>
+        <i val="false"/>
+        <strike val="false"/>
+        <color rgb="FFFFFFFF"/>
+        <sz val="7"/>
+        <u val="none"/>
+      </rPr>
+      <t xml:space="preserve">Hora: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="false"/>
+        <i val="false"/>
+        <strike val="false"/>
+        <color rgb="FFFFFFFF"/>
+        <sz val="7"/>
+        <u val="none"/>
+      </rPr>
+      <t xml:space="preserve">10:40
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="true"/>
+        <i val="false"/>
+        <strike val="false"/>
+        <color rgb="FFFFFFFF"/>
+        <sz val="7"/>
+        <u val="none"/>
+      </rPr>
+      <t xml:space="preserve">Fecha: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="false"/>
+        <i val="false"/>
+        <strike val="false"/>
+        <color rgb="FFFFFFFF"/>
+        <sz val="7"/>
+        <u val="none"/>
+      </rPr>
+      <t xml:space="preserve">30-06-2025
+</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="true"/>
+        <i val="false"/>
+        <strike val="false"/>
+        <color rgb="FFFFFFFF"/>
+        <sz val="7"/>
+        <u val="none"/>
+      </rPr>
+      <t xml:space="preserve">Usuario: </t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Calibri"/>
+        <b val="false"/>
+        <i val="false"/>
+        <strike val="false"/>
+        <color rgb="FFFFFFFF"/>
+        <sz val="7"/>
+        <u val="none"/>
+      </rPr>
+      <t xml:space="preserve">Jean Pierre Asencio</t>
+    </r>
+  </si>
+  <si>
+    <t>MODULOS DE SUBCUENTA DE BLOQUE</t>
+  </si>
+  <si>
+    <t>CUENTA:1.1.01.01.10.01    FONDOS GASTOS DE VIAJE</t>
+  </si>
+  <si>
+    <t>GRUPO:0502280092-ABAD JOEL</t>
+  </si>
+  <si>
+    <t>Mayor de Submódulo:Cta. por Cobrar</t>
+  </si>
+  <si>
+    <t>Saldo Anterior S/</t>
+  </si>
+  <si>
+    <t>FECHA</t>
+  </si>
+  <si>
+    <t>FACTURA</t>
+  </si>
+  <si>
+    <t>TD</t>
+  </si>
+  <si>
+    <t>NUMERO</t>
+  </si>
+  <si>
+    <t>CO N C E P T O</t>
+  </si>
+  <si>
+    <t>PARCIAL M/E</t>
+  </si>
+  <si>
+    <t>DEBITOS</t>
+  </si>
+  <si>
+    <t>CREDITOS</t>
+  </si>
+  <si>
+    <t>SALDO</t>
+  </si>
+  <si>
+    <t>2025-02-27</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>2000003</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>T o t a l e s</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -25,7 +167,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -36,7 +178,16 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <b val="0"/>
+      <b val="1"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="1"/>
       <i val="0"/>
       <strike val="0"/>
       <u val="none"/>
@@ -45,7 +196,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -55,19 +206,58 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <gradientFill type="linear" degree="90">
+        <stop position="0">
+          <color rgb="FF436BEE"/>
+        </stop>
+        <stop position="1">
+          <color rgb="FFFFFFFF"/>
+        </stop>
+      </gradientFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF436BEE"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border/>
+    <border>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="2" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="3" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="2" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
+    <xf xfId="0" fontId="0" numFmtId="2" fillId="0" borderId="0" applyFont="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
     <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="0" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -112,7 +302,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>857250</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -433,26 +623,235 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="100" customWidth="true" style="0"/>
-    <col min="2" max="2" width="40" customWidth="true" style="0"/>
+    <col min="1" max="1" width="15" customWidth="true" style="0"/>
+    <col min="2" max="2" width="15" customWidth="true" style="0"/>
+    <col min="3" max="3" width="8" customWidth="true" style="0"/>
+    <col min="4" max="4" width="15" customWidth="true" style="0"/>
+    <col min="5" max="5" width="69" customWidth="true" style="0"/>
+    <col min="6" max="6" width="20" customWidth="true" style="0"/>
+    <col min="7" max="7" width="15" customWidth="true" style="0"/>
+    <col min="8" max="8" width="15" customWidth="true" style="0"/>
+    <col min="9" max="9" width="15" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" customHeight="1" ht="45">
-      <c r="A1"/>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:9" customHeight="1" ht="45">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <rFont val="Calibri"/>
+              <b val="true"/>
+              <i val="false"/>
+              <strike val="false"/>
+              <color rgb="FFFFFFFF"/>
+              <sz val="7"/>
+              <u val="none"/>
+            </rPr>
+            <t xml:space="preserve">Hora: </t>
+          </r>
+          <r>
+            <rPr>
+              <rFont val="Calibri"/>
+              <b val="false"/>
+              <i val="false"/>
+              <strike val="false"/>
+              <color rgb="FFFFFFFF"/>
+              <sz val="7"/>
+              <u val="none"/>
+            </rPr>
+            <t xml:space="preserve">10:40
+</t>
+          </r>
+          <r>
+            <rPr>
+              <rFont val="Calibri"/>
+              <b val="true"/>
+              <i val="false"/>
+              <strike val="false"/>
+              <color rgb="FFFFFFFF"/>
+              <sz val="7"/>
+              <u val="none"/>
+            </rPr>
+            <t xml:space="preserve">Fecha: </t>
+          </r>
+          <r>
+            <rPr>
+              <rFont val="Calibri"/>
+              <b val="false"/>
+              <i val="false"/>
+              <strike val="false"/>
+              <color rgb="FFFFFFFF"/>
+              <sz val="7"/>
+              <u val="none"/>
+            </rPr>
+            <t xml:space="preserve">30-06-2025
+</t>
+          </r>
+          <r>
+            <rPr>
+              <rFont val="Calibri"/>
+              <b val="true"/>
+              <i val="false"/>
+              <strike val="false"/>
+              <color rgb="FFFFFFFF"/>
+              <sz val="7"/>
+              <u val="none"/>
+            </rPr>
+            <t xml:space="preserve">Usuario: </t>
+          </r>
+          <r>
+            <rPr>
+              <rFont val="Calibri"/>
+              <b val="false"/>
+              <i val="false"/>
+              <strike val="false"/>
+              <color rgb="FFFFFFFF"/>
+              <sz val="7"/>
+              <u val="none"/>
+            </rPr>
+            <t xml:space="preserve">Jean Pierre Asencio</t>
+          </r>
+        </is>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="G6" s="6">
+        <v>10.0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="I6" s="6">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="E4:I4"/>
+  </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>

</xml_diff>